<commit_message>
Update fee collection and reports with recent transactions
Added new fee payment records and updated fee status for multiple students in daywise, yearwise, and transaction reports. Adjusted class/section assignments and corrected payment details in several CSV files to reflect recent collections and corrections. Binary report and dashboard files were also updated to include the latest data.
</commit_message>
<xml_diff>
--- a/output_data/atom_report.xlsx
+++ b/output_data/atom_report.xlsx
@@ -16573,310 +16573,3658 @@
       </c>
       <c r="M45" t="inlineStr">
         <is>
+          <t>RS</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>531128921024</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t>100000036600</t>
+        </is>
+      </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>SIBL0000899</t>
+        </is>
+      </c>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>10-Nov-2025 00:00:00</t>
+        </is>
+      </c>
+      <c r="S45" t="inlineStr">
+        <is>
+          <t>MERCHANT</t>
+        </is>
+      </c>
+      <c r="T45" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="U45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X45" t="inlineStr">
+        <is>
+          <t>PENAKADITHI SAMUEL</t>
+        </is>
+      </c>
+      <c r="Y45" t="inlineStr">
+        <is>
+          <t>kotakschoolvsp@gmail.com</t>
+        </is>
+      </c>
+      <c r="Z45" t="inlineStr">
+        <is>
+          <t>9030736744</t>
+        </is>
+      </c>
+      <c r="AA45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG45" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AH45" t="inlineStr">
+        <is>
+          <t>0.9</t>
+        </is>
+      </c>
+      <c r="AI45" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AJ45" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AK45" t="inlineStr">
+        <is>
+          <t>5.9</t>
+        </is>
+      </c>
+      <c r="AL45" t="inlineStr">
+        <is>
+          <t>6750.0</t>
+        </is>
+      </c>
+      <c r="AM45" t="inlineStr">
+        <is>
+          <t>10-Nov-2025 00:00:00</t>
+        </is>
+      </c>
+      <c r="AN45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT45" t="inlineStr">
+        <is>
+          <t>TRANSACTION IS SUCCESSFUL</t>
+        </is>
+      </c>
+      <c r="AU45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA45" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="BB45" t="inlineStr">
+        <is>
+          <t>KOTAK SALESIAN SCHOOL MANAGEMENT ACCOUNT</t>
+        </is>
+      </c>
+      <c r="BC45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BD45" t="inlineStr">
+        <is>
+          <t>REGULAR</t>
+        </is>
+      </c>
+      <c r="BE45" t="inlineStr">
+        <is>
+          <t>19989</t>
+        </is>
+      </c>
+      <c r="BF45" t="inlineStr">
+        <is>
+          <t>265141</t>
+        </is>
+      </c>
+      <c r="BG45" t="inlineStr">
+        <is>
+          <t>2047</t>
+        </is>
+      </c>
+      <c r="BH45" t="inlineStr">
+        <is>
+          <t>six thousand seven hundred fifty</t>
+        </is>
+      </c>
+      <c r="BI45" t="inlineStr">
+        <is>
+          <t>17278</t>
+        </is>
+      </c>
+      <c r="BJ45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BK45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BL45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BM45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BN45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BO45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BP45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BQ45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BR45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BS45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BT45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BU45" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="BV45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>SALESIAN EDUCATION SOCIETY</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>753702</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>11000315754150</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>1762746971</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>8350.00</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>10-Nov-2025 09:27:15</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>lVl</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>sale</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>ICICI UPI QR</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>RS</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>531445403467</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t>100000036600</t>
+        </is>
+      </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>SIBL0000899</t>
+        </is>
+      </c>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>11-Nov-2025 00:00:00</t>
+        </is>
+      </c>
+      <c r="S46" t="inlineStr">
+        <is>
+          <t>MERCHANT</t>
+        </is>
+      </c>
+      <c r="T46" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X46" t="inlineStr">
+        <is>
+          <t>KARRI ABHINAY CHARVIK</t>
+        </is>
+      </c>
+      <c r="Y46" t="inlineStr">
+        <is>
+          <t>kotakschoolvsp@gmail.com</t>
+        </is>
+      </c>
+      <c r="Z46" t="inlineStr">
+        <is>
+          <t>9177965994</t>
+        </is>
+      </c>
+      <c r="AA46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG46" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AH46" t="inlineStr">
+        <is>
+          <t>0.9</t>
+        </is>
+      </c>
+      <c r="AI46" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AJ46" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AK46" t="inlineStr">
+        <is>
+          <t>5.9</t>
+        </is>
+      </c>
+      <c r="AL46" t="inlineStr">
+        <is>
+          <t>8350.0</t>
+        </is>
+      </c>
+      <c r="AM46" t="inlineStr">
+        <is>
+          <t>11-Nov-2025 00:00:00</t>
+        </is>
+      </c>
+      <c r="AN46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT46" t="inlineStr">
+        <is>
+          <t>TRANSACTION IS SUCCESSFUL</t>
+        </is>
+      </c>
+      <c r="AU46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA46" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="BB46" t="inlineStr">
+        <is>
+          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
+        </is>
+      </c>
+      <c r="BC46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BD46" t="inlineStr">
+        <is>
+          <t>REGULAR</t>
+        </is>
+      </c>
+      <c r="BE46" t="inlineStr">
+        <is>
+          <t>18807</t>
+        </is>
+      </c>
+      <c r="BF46" t="inlineStr">
+        <is>
+          <t>265833</t>
+        </is>
+      </c>
+      <c r="BG46" t="inlineStr">
+        <is>
+          <t>2050</t>
+        </is>
+      </c>
+      <c r="BH46" t="inlineStr">
+        <is>
+          <t>eight thousand three hundred fifty</t>
+        </is>
+      </c>
+      <c r="BI46" t="inlineStr">
+        <is>
+          <t>16104</t>
+        </is>
+      </c>
+      <c r="BJ46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BK46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BL46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BM46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BN46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BO46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BP46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BQ46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BR46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BS46" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BT46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BU46" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="BV46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>SALESIAN EDUCATION SOCIETY</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>753702</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>11000316004290</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>1762781636</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>8550.00</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>10-Nov-2025 19:06:39</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>lVl</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>sale</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>ICICI UPI QR</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
           <t>NRNS</t>
         </is>
       </c>
-      <c r="N45" t="inlineStr">
-        <is>
-          <t>531128921024</t>
-        </is>
-      </c>
-      <c r="O45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P45" t="inlineStr">
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>531448759161</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P47" t="inlineStr">
         <is>
           <t>100000036600</t>
         </is>
       </c>
-      <c r="Q45" t="inlineStr">
+      <c r="Q47" t="inlineStr">
         <is>
           <t>SIBL0000899</t>
         </is>
       </c>
-      <c r="R45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="S45" t="inlineStr">
+      <c r="R47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S47" t="inlineStr">
         <is>
           <t>MERCHANT</t>
         </is>
       </c>
-      <c r="T45" t="inlineStr">
+      <c r="T47" t="inlineStr">
         <is>
           <t>UPI</t>
         </is>
       </c>
-      <c r="U45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="V45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="W45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="X45" t="inlineStr">
-        <is>
-          <t>PENAKADITHI SAMUEL</t>
-        </is>
-      </c>
-      <c r="Y45" t="inlineStr">
+      <c r="U47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X47" t="inlineStr">
+        <is>
+          <t>NITHYA EMERALD THOTA</t>
+        </is>
+      </c>
+      <c r="Y47" t="inlineStr">
         <is>
           <t>kotakschoolvsp@gmail.com</t>
         </is>
       </c>
-      <c r="Z45" t="inlineStr">
-        <is>
-          <t>9030736744</t>
-        </is>
-      </c>
-      <c r="AA45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AB45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AC45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AD45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AE45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AF45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AG45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AH45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AI45" t="inlineStr">
+      <c r="Z47" t="inlineStr">
+        <is>
+          <t>8919560551</t>
+        </is>
+      </c>
+      <c r="AA47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI47" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="AJ45" t="inlineStr">
+      <c r="AJ47" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="AK45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AL45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AM45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AN45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AO45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AP45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AQ45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AR45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AS45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AT45" t="inlineStr">
+      <c r="AK47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT47" t="inlineStr">
+        <is>
+          <t>TRANSACTION IS FAILED</t>
+        </is>
+      </c>
+      <c r="AU47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA47" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="BB47" t="inlineStr">
+        <is>
+          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
+        </is>
+      </c>
+      <c r="BC47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BD47" t="inlineStr">
+        <is>
+          <t>REGULAR</t>
+        </is>
+      </c>
+      <c r="BE47" t="inlineStr">
+        <is>
+          <t>18526</t>
+        </is>
+      </c>
+      <c r="BF47" t="inlineStr">
+        <is>
+          <t>262171,263959</t>
+        </is>
+      </c>
+      <c r="BG47" t="inlineStr">
+        <is>
+          <t>2037,2041</t>
+        </is>
+      </c>
+      <c r="BH47" t="inlineStr">
+        <is>
+          <t>eight thousand five hundred fifty</t>
+        </is>
+      </c>
+      <c r="BI47" t="inlineStr">
+        <is>
+          <t>16983</t>
+        </is>
+      </c>
+      <c r="BJ47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BK47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BL47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BM47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BN47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BO47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BP47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BQ47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BR47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BS47" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BT47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BU47" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="BV47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>SALESIAN EDUCATION SOCIETY</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>753702</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>11000316031833</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>1762789270</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>10750.00</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>10-Nov-2025 21:12:45</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>VlllX</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>sale</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>ICICI UPI QR</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>NRNS</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>531449475884</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>100000036600</t>
+        </is>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>SIBL0000899</t>
+        </is>
+      </c>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S48" t="inlineStr">
+        <is>
+          <t>MERCHANT</t>
+        </is>
+      </c>
+      <c r="T48" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="U48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X48" t="inlineStr">
+        <is>
+          <t>GURRALA RUSHABH NARAYAN</t>
+        </is>
+      </c>
+      <c r="Y48" t="inlineStr">
+        <is>
+          <t>kotakschoolvsp@gmail.com</t>
+        </is>
+      </c>
+      <c r="Z48" t="inlineStr">
+        <is>
+          <t>9704995001</t>
+        </is>
+      </c>
+      <c r="AA48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI48" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AJ48" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AK48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT48" t="inlineStr">
+        <is>
+          <t>TRANSACTION IS FAILED</t>
+        </is>
+      </c>
+      <c r="AU48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA48" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="BB48" t="inlineStr">
+        <is>
+          <t>KOTAK SALESIAN SECONDARY SCHOOL ICSE</t>
+        </is>
+      </c>
+      <c r="BC48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BD48" t="inlineStr">
+        <is>
+          <t>REGULAR</t>
+        </is>
+      </c>
+      <c r="BE48" t="inlineStr">
+        <is>
+          <t>19325</t>
+        </is>
+      </c>
+      <c r="BF48" t="inlineStr">
+        <is>
+          <t>266322</t>
+        </is>
+      </c>
+      <c r="BG48" t="inlineStr">
+        <is>
+          <t>2052</t>
+        </is>
+      </c>
+      <c r="BH48" t="inlineStr">
+        <is>
+          <t>ten thousand seven hundred fifty</t>
+        </is>
+      </c>
+      <c r="BI48" t="inlineStr">
+        <is>
+          <t>16052</t>
+        </is>
+      </c>
+      <c r="BJ48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BK48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BL48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BM48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BN48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BO48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BP48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BQ48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BR48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BS48" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BT48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BU48" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="BV48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>SALESIAN EDUCATION SOCIETY</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>753702</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>11000316033651</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>1762789270</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>10750.00</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>10-Nov-2025 21:17:01</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>VlllX</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>sale</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>ICICI UPI QR</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>RNS</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>531449495645</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>100000036600</t>
+        </is>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>SIBL0000899</t>
+        </is>
+      </c>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S49" t="inlineStr">
+        <is>
+          <t>MERCHANT</t>
+        </is>
+      </c>
+      <c r="T49" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="U49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X49" t="inlineStr">
+        <is>
+          <t>GURRALA RUSHABH NARAYAN</t>
+        </is>
+      </c>
+      <c r="Y49" t="inlineStr">
+        <is>
+          <t>kotakschoolvsp@gmail.com</t>
+        </is>
+      </c>
+      <c r="Z49" t="inlineStr">
+        <is>
+          <t>9704995001</t>
+        </is>
+      </c>
+      <c r="AA49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG49" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AH49" t="inlineStr">
+        <is>
+          <t>0.9</t>
+        </is>
+      </c>
+      <c r="AI49" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AJ49" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AK49" t="inlineStr">
+        <is>
+          <t>5.9</t>
+        </is>
+      </c>
+      <c r="AL49" t="inlineStr">
+        <is>
+          <t>10750.0</t>
+        </is>
+      </c>
+      <c r="AM49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT49" t="inlineStr">
         <is>
           <t>TRANSACTION IS SUCCESSFUL</t>
         </is>
       </c>
-      <c r="AU45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AV45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AW45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AX45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AY45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AZ45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BA45" t="inlineStr">
+      <c r="AU49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA49" t="inlineStr">
         <is>
           <t>UPI</t>
         </is>
       </c>
-      <c r="BB45" t="inlineStr">
+      <c r="BB49" t="inlineStr">
+        <is>
+          <t>KOTAK SALESIAN SECONDARY SCHOOL ICSE</t>
+        </is>
+      </c>
+      <c r="BC49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BD49" t="inlineStr">
+        <is>
+          <t>REGULAR</t>
+        </is>
+      </c>
+      <c r="BE49" t="inlineStr">
+        <is>
+          <t>19325</t>
+        </is>
+      </c>
+      <c r="BF49" t="inlineStr">
+        <is>
+          <t>266322</t>
+        </is>
+      </c>
+      <c r="BG49" t="inlineStr">
+        <is>
+          <t>2052</t>
+        </is>
+      </c>
+      <c r="BH49" t="inlineStr">
+        <is>
+          <t>ten thousand seven hundred fifty</t>
+        </is>
+      </c>
+      <c r="BI49" t="inlineStr">
+        <is>
+          <t>16052</t>
+        </is>
+      </c>
+      <c r="BJ49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BK49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BL49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BM49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BN49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BO49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BP49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BQ49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BR49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BS49" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BT49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BU49" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="BV49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>SALESIAN EDUCATION SOCIETY</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>753702</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>11000316067938</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>1762821403</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>6750.00</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>11-Nov-2025 05:53:50</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>PREKGUKG</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>sale</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>ICICI UPI QR</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>NRNS</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>030020732085</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t>100000036600</t>
+        </is>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>SIBL0000899</t>
+        </is>
+      </c>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S50" t="inlineStr">
+        <is>
+          <t>MERCHANT</t>
+        </is>
+      </c>
+      <c r="T50" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X50" t="inlineStr">
+        <is>
+          <t>VADIGI DIVYESH SAI PAVAN</t>
+        </is>
+      </c>
+      <c r="Y50" t="inlineStr">
+        <is>
+          <t>kotakschoolvsp@gmail.com</t>
+        </is>
+      </c>
+      <c r="Z50" t="inlineStr">
+        <is>
+          <t>8367352524</t>
+        </is>
+      </c>
+      <c r="AA50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI50" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AJ50" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AK50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT50" t="inlineStr">
+        <is>
+          <t>TRANSACTION IS SUCCESSFUL</t>
+        </is>
+      </c>
+      <c r="AU50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA50" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="BB50" t="inlineStr">
         <is>
           <t>KOTAK SALESIAN SCHOOL MANAGEMENT ACCOUNT</t>
         </is>
       </c>
-      <c r="BC45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BD45" t="inlineStr">
+      <c r="BC50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BD50" t="inlineStr">
         <is>
           <t>REGULAR</t>
         </is>
       </c>
-      <c r="BE45" t="inlineStr">
-        <is>
-          <t>19989</t>
-        </is>
-      </c>
-      <c r="BF45" t="inlineStr">
-        <is>
-          <t>265141</t>
-        </is>
-      </c>
-      <c r="BG45" t="inlineStr">
+      <c r="BE50" t="inlineStr">
+        <is>
+          <t>20023</t>
+        </is>
+      </c>
+      <c r="BF50" t="inlineStr">
+        <is>
+          <t>265150</t>
+        </is>
+      </c>
+      <c r="BG50" t="inlineStr">
         <is>
           <t>2047</t>
         </is>
       </c>
-      <c r="BH45" t="inlineStr">
+      <c r="BH50" t="inlineStr">
         <is>
           <t>six thousand seven hundred fifty</t>
         </is>
       </c>
-      <c r="BI45" t="inlineStr">
-        <is>
-          <t>17278</t>
-        </is>
-      </c>
-      <c r="BJ45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BK45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BL45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BM45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BN45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BO45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BP45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BQ45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BR45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BS45" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BT45" t="inlineStr">
+      <c r="BI50" t="inlineStr">
+        <is>
+          <t>17315</t>
+        </is>
+      </c>
+      <c r="BJ50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BK50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BL50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BM50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BN50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BO50" t="inlineStr">
+        <is>
+          <t>UPI INTENT</t>
+        </is>
+      </c>
+      <c r="BP50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BQ50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BR50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BS50" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BT50" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="BU45" t="inlineStr">
+      <c r="BU50" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="BV45" t="inlineStr">
+      <c r="BV50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>SALESIAN EDUCATION SOCIETY</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>753702</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>11000316099462</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>1762835725</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>8350.00</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>11-Nov-2025 10:09:11</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>lVl</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>sale</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>ICICI UPI QR</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>NRNS</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>108551696284</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t>100000036600</t>
+        </is>
+      </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>SIBL0000899</t>
+        </is>
+      </c>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S51" t="inlineStr">
+        <is>
+          <t>MERCHANT</t>
+        </is>
+      </c>
+      <c r="T51" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="U51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X51" t="inlineStr">
+        <is>
+          <t>HARINI CHAND REDDY PILAKA</t>
+        </is>
+      </c>
+      <c r="Y51" t="inlineStr">
+        <is>
+          <t>kotakschoolvsp@gmail.com</t>
+        </is>
+      </c>
+      <c r="Z51" t="inlineStr">
+        <is>
+          <t>9866815664</t>
+        </is>
+      </c>
+      <c r="AA51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI51" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AJ51" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AK51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT51" t="inlineStr">
+        <is>
+          <t>TRANSACTION IS SUCCESSFUL</t>
+        </is>
+      </c>
+      <c r="AU51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA51" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="BB51" t="inlineStr">
+        <is>
+          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
+        </is>
+      </c>
+      <c r="BC51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BD51" t="inlineStr">
+        <is>
+          <t>REGULAR</t>
+        </is>
+      </c>
+      <c r="BE51" t="inlineStr">
+        <is>
+          <t>18753</t>
+        </is>
+      </c>
+      <c r="BF51" t="inlineStr">
+        <is>
+          <t>265774</t>
+        </is>
+      </c>
+      <c r="BG51" t="inlineStr">
+        <is>
+          <t>2050</t>
+        </is>
+      </c>
+      <c r="BH51" t="inlineStr">
+        <is>
+          <t>eight thousand three hundred fifty</t>
+        </is>
+      </c>
+      <c r="BI51" t="inlineStr">
+        <is>
+          <t>16733</t>
+        </is>
+      </c>
+      <c r="BJ51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BK51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BL51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BM51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BN51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BO51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BP51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BQ51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BR51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BS51" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BT51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BU51" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="BV51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>SALESIAN EDUCATION SOCIETY</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>753702</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>11000316100223</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>1762836014</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>11350.00</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>11-Nov-2025 10:10:40</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>VlllX</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>sale</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>ICICI UPI QR</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>NRNS</t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>108551703754</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t>100000036600</t>
+        </is>
+      </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>SIBL0000899</t>
+        </is>
+      </c>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S52" t="inlineStr">
+        <is>
+          <t>MERCHANT</t>
+        </is>
+      </c>
+      <c r="T52" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="U52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X52" t="inlineStr">
+        <is>
+          <t>HASINI CHAND REDDY PILAKA</t>
+        </is>
+      </c>
+      <c r="Y52" t="inlineStr">
+        <is>
+          <t>kotakschoolvsp@gmail.com</t>
+        </is>
+      </c>
+      <c r="Z52" t="inlineStr">
+        <is>
+          <t>9866815664</t>
+        </is>
+      </c>
+      <c r="AA52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI52" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AJ52" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AK52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT52" t="inlineStr">
+        <is>
+          <t>TRANSACTION IS SUCCESSFUL</t>
+        </is>
+      </c>
+      <c r="AU52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA52" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="BB52" t="inlineStr">
+        <is>
+          <t>KOTAK SALESIAN SECONDARY SCHOOL ICSE</t>
+        </is>
+      </c>
+      <c r="BC52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BD52" t="inlineStr">
+        <is>
+          <t>REGULAR</t>
+        </is>
+      </c>
+      <c r="BE52" t="inlineStr">
+        <is>
+          <t>19425</t>
+        </is>
+      </c>
+      <c r="BF52" t="inlineStr">
+        <is>
+          <t>266398</t>
+        </is>
+      </c>
+      <c r="BG52" t="inlineStr">
+        <is>
+          <t>2053</t>
+        </is>
+      </c>
+      <c r="BH52" t="inlineStr">
+        <is>
+          <t>eleven thousand three hundred fifty</t>
+        </is>
+      </c>
+      <c r="BI52" t="inlineStr">
+        <is>
+          <t>16734</t>
+        </is>
+      </c>
+      <c r="BJ52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BK52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BL52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BM52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BN52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BO52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BP52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BQ52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BR52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BS52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BT52" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BU52" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="BV52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>SALESIAN EDUCATION SOCIETY</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>753702</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>11000316192344</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>1762858254</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>6750.00</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>11-Nov-2025 16:21:09</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>PREKGUKG</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>sale</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>ICICI UPI QR</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>NRNS</t>
+        </is>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>704447957133</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P53" t="inlineStr">
+        <is>
+          <t>100000036600</t>
+        </is>
+      </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>SIBL0000899</t>
+        </is>
+      </c>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S53" t="inlineStr">
+        <is>
+          <t>MERCHANT</t>
+        </is>
+      </c>
+      <c r="T53" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="U53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X53" t="inlineStr">
+        <is>
+          <t>THUTTA HARI CHARANI</t>
+        </is>
+      </c>
+      <c r="Y53" t="inlineStr">
+        <is>
+          <t>kotakschoolvsp@gmail.com</t>
+        </is>
+      </c>
+      <c r="Z53" t="inlineStr">
+        <is>
+          <t>7337239208</t>
+        </is>
+      </c>
+      <c r="AA53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI53" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AJ53" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AK53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT53" t="inlineStr">
+        <is>
+          <t>TRANSACTION IS SUCCESSFUL</t>
+        </is>
+      </c>
+      <c r="AU53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA53" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="BB53" t="inlineStr">
+        <is>
+          <t>KOTAK SALESIAN SCHOOL MANAGEMENT ACCOUNT</t>
+        </is>
+      </c>
+      <c r="BC53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BD53" t="inlineStr">
+        <is>
+          <t>REGULAR</t>
+        </is>
+      </c>
+      <c r="BE53" t="inlineStr">
+        <is>
+          <t>19892</t>
+        </is>
+      </c>
+      <c r="BF53" t="inlineStr">
+        <is>
+          <t>265011</t>
+        </is>
+      </c>
+      <c r="BG53" t="inlineStr">
+        <is>
+          <t>2047</t>
+        </is>
+      </c>
+      <c r="BH53" t="inlineStr">
+        <is>
+          <t>six thousand seven hundred fifty</t>
+        </is>
+      </c>
+      <c r="BI53" t="inlineStr">
+        <is>
+          <t>17177</t>
+        </is>
+      </c>
+      <c r="BJ53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BK53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BL53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BM53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BN53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BO53" t="inlineStr">
+        <is>
+          <t>UPI INTENT</t>
+        </is>
+      </c>
+      <c r="BP53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BQ53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BR53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BS53" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BT53" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BU53" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="BV53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>SALESIAN EDUCATION SOCIETY</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>753702</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>11000316191666</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>1762858305</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>7750.00</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>11-Nov-2025 16:21:56</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>lVl</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>sale</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>ICICI UPI QR</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>NRNS</t>
+        </is>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>783823510579</t>
+        </is>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t>100000036600</t>
+        </is>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>SIBL0000899</t>
+        </is>
+      </c>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S54" t="inlineStr">
+        <is>
+          <t>MERCHANT</t>
+        </is>
+      </c>
+      <c r="T54" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="U54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X54" t="inlineStr">
+        <is>
+          <t>THUTTA DHANASHVI</t>
+        </is>
+      </c>
+      <c r="Y54" t="inlineStr">
+        <is>
+          <t>kotakschoolvsp@gmail.com</t>
+        </is>
+      </c>
+      <c r="Z54" t="inlineStr">
+        <is>
+          <t>7337239208</t>
+        </is>
+      </c>
+      <c r="AA54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI54" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AJ54" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AK54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT54" t="inlineStr">
+        <is>
+          <t>TRANSACTION IS SUCCESSFUL</t>
+        </is>
+      </c>
+      <c r="AU54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA54" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="BB54" t="inlineStr">
+        <is>
+          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
+        </is>
+      </c>
+      <c r="BC54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BD54" t="inlineStr">
+        <is>
+          <t>REGULAR</t>
+        </is>
+      </c>
+      <c r="BE54" t="inlineStr">
+        <is>
+          <t>18339</t>
+        </is>
+      </c>
+      <c r="BF54" t="inlineStr">
+        <is>
+          <t>265347</t>
+        </is>
+      </c>
+      <c r="BG54" t="inlineStr">
+        <is>
+          <t>2048</t>
+        </is>
+      </c>
+      <c r="BH54" t="inlineStr">
+        <is>
+          <t>seven thousand seven hundred fifty</t>
+        </is>
+      </c>
+      <c r="BI54" t="inlineStr">
+        <is>
+          <t>16927</t>
+        </is>
+      </c>
+      <c r="BJ54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BK54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BL54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BM54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BN54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BO54" t="inlineStr">
+        <is>
+          <t>UPI INTENT</t>
+        </is>
+      </c>
+      <c r="BP54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BQ54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BR54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BS54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BT54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BU54" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="BV54" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
Update fee collection and reports with new payments
Added new fee payment records for multiple students in daywise and 2025-26 fee collection CSVs. Updated fee status and payment details in fees_collection.csv and fees_report.csv to reflect recent payments. Also updated related Excel and Power BI dashboard files to ensure consistency across reports.
</commit_message>
<xml_diff>
--- a/output_data/atom_report.xlsx
+++ b/output_data/atom_report.xlsx
@@ -18433,7 +18433,7 @@
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>NRNS</t>
+          <t>RS</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
@@ -18458,7 +18458,7 @@
       </c>
       <c r="R50" t="inlineStr">
         <is>
-          <t/>
+          <t>12-Nov-2025 00:00:00</t>
         </is>
       </c>
       <c r="S50" t="inlineStr">
@@ -18533,12 +18533,12 @@
       </c>
       <c r="AG50" t="inlineStr">
         <is>
-          <t/>
+          <t>5</t>
         </is>
       </c>
       <c r="AH50" t="inlineStr">
         <is>
-          <t/>
+          <t>0.9</t>
         </is>
       </c>
       <c r="AI50" t="inlineStr">
@@ -18553,17 +18553,17 @@
       </c>
       <c r="AK50" t="inlineStr">
         <is>
-          <t/>
+          <t>5.9</t>
         </is>
       </c>
       <c r="AL50" t="inlineStr">
         <is>
-          <t/>
+          <t>6750.0</t>
         </is>
       </c>
       <c r="AM50" t="inlineStr">
         <is>
-          <t/>
+          <t>12-Nov-2025 00:00:00</t>
         </is>
       </c>
       <c r="AN50" t="inlineStr">
@@ -18805,7 +18805,7 @@
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>NRNS</t>
+          <t>RS</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
@@ -18830,7 +18830,7 @@
       </c>
       <c r="R51" t="inlineStr">
         <is>
-          <t/>
+          <t>12-Nov-2025 00:00:00</t>
         </is>
       </c>
       <c r="S51" t="inlineStr">
@@ -18905,12 +18905,12 @@
       </c>
       <c r="AG51" t="inlineStr">
         <is>
-          <t/>
+          <t>5</t>
         </is>
       </c>
       <c r="AH51" t="inlineStr">
         <is>
-          <t/>
+          <t>0.9</t>
         </is>
       </c>
       <c r="AI51" t="inlineStr">
@@ -18925,17 +18925,17 @@
       </c>
       <c r="AK51" t="inlineStr">
         <is>
-          <t/>
+          <t>5.9</t>
         </is>
       </c>
       <c r="AL51" t="inlineStr">
         <is>
-          <t/>
+          <t>8350.0</t>
         </is>
       </c>
       <c r="AM51" t="inlineStr">
         <is>
-          <t/>
+          <t>12-Nov-2025 00:00:00</t>
         </is>
       </c>
       <c r="AN51" t="inlineStr">
@@ -19177,7 +19177,7 @@
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>NRNS</t>
+          <t>RNS</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
@@ -19277,12 +19277,12 @@
       </c>
       <c r="AG52" t="inlineStr">
         <is>
-          <t/>
+          <t>5</t>
         </is>
       </c>
       <c r="AH52" t="inlineStr">
         <is>
-          <t/>
+          <t>0.9</t>
         </is>
       </c>
       <c r="AI52" t="inlineStr">
@@ -19297,12 +19297,12 @@
       </c>
       <c r="AK52" t="inlineStr">
         <is>
-          <t/>
+          <t>5.9</t>
         </is>
       </c>
       <c r="AL52" t="inlineStr">
         <is>
-          <t/>
+          <t>11350.0</t>
         </is>
       </c>
       <c r="AM52" t="inlineStr">
@@ -19549,7 +19549,7 @@
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>NRNS</t>
+          <t>RS</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
@@ -19574,7 +19574,7 @@
       </c>
       <c r="R53" t="inlineStr">
         <is>
-          <t/>
+          <t>12-Nov-2025 00:00:00</t>
         </is>
       </c>
       <c r="S53" t="inlineStr">
@@ -19649,12 +19649,12 @@
       </c>
       <c r="AG53" t="inlineStr">
         <is>
-          <t/>
+          <t>5</t>
         </is>
       </c>
       <c r="AH53" t="inlineStr">
         <is>
-          <t/>
+          <t>0.9</t>
         </is>
       </c>
       <c r="AI53" t="inlineStr">
@@ -19669,17 +19669,17 @@
       </c>
       <c r="AK53" t="inlineStr">
         <is>
-          <t/>
+          <t>5.9</t>
         </is>
       </c>
       <c r="AL53" t="inlineStr">
         <is>
-          <t/>
+          <t>6750.0</t>
         </is>
       </c>
       <c r="AM53" t="inlineStr">
         <is>
-          <t/>
+          <t>12-Nov-2025 00:00:00</t>
         </is>
       </c>
       <c r="AN53" t="inlineStr">
@@ -19921,310 +19921,1054 @@
       </c>
       <c r="M54" t="inlineStr">
         <is>
+          <t>RS</t>
+        </is>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>783823510579</t>
+        </is>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t>100000036600</t>
+        </is>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>SIBL0000899</t>
+        </is>
+      </c>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>12-Nov-2025 00:00:00</t>
+        </is>
+      </c>
+      <c r="S54" t="inlineStr">
+        <is>
+          <t>MERCHANT</t>
+        </is>
+      </c>
+      <c r="T54" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="U54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X54" t="inlineStr">
+        <is>
+          <t>THUTTA DHANASHVI</t>
+        </is>
+      </c>
+      <c r="Y54" t="inlineStr">
+        <is>
+          <t>kotakschoolvsp@gmail.com</t>
+        </is>
+      </c>
+      <c r="Z54" t="inlineStr">
+        <is>
+          <t>7337239208</t>
+        </is>
+      </c>
+      <c r="AA54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG54" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AH54" t="inlineStr">
+        <is>
+          <t>0.9</t>
+        </is>
+      </c>
+      <c r="AI54" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AJ54" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AK54" t="inlineStr">
+        <is>
+          <t>5.9</t>
+        </is>
+      </c>
+      <c r="AL54" t="inlineStr">
+        <is>
+          <t>7750.0</t>
+        </is>
+      </c>
+      <c r="AM54" t="inlineStr">
+        <is>
+          <t>12-Nov-2025 00:00:00</t>
+        </is>
+      </c>
+      <c r="AN54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT54" t="inlineStr">
+        <is>
+          <t>TRANSACTION IS SUCCESSFUL</t>
+        </is>
+      </c>
+      <c r="AU54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA54" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="BB54" t="inlineStr">
+        <is>
+          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
+        </is>
+      </c>
+      <c r="BC54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BD54" t="inlineStr">
+        <is>
+          <t>REGULAR</t>
+        </is>
+      </c>
+      <c r="BE54" t="inlineStr">
+        <is>
+          <t>18339</t>
+        </is>
+      </c>
+      <c r="BF54" t="inlineStr">
+        <is>
+          <t>265347</t>
+        </is>
+      </c>
+      <c r="BG54" t="inlineStr">
+        <is>
+          <t>2048</t>
+        </is>
+      </c>
+      <c r="BH54" t="inlineStr">
+        <is>
+          <t>seven thousand seven hundred fifty</t>
+        </is>
+      </c>
+      <c r="BI54" t="inlineStr">
+        <is>
+          <t>16927</t>
+        </is>
+      </c>
+      <c r="BJ54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BK54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BL54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BM54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BN54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BO54" t="inlineStr">
+        <is>
+          <t>UPI INTENT</t>
+        </is>
+      </c>
+      <c r="BP54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BQ54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BR54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BS54" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BT54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BU54" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="BV54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>SALESIAN EDUCATION SOCIETY</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>753702</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>11000316275259</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>1762918783</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>6750.00</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>12-Nov-2025 09:11:42</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>PREKGUKG</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>sale</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>ICICI UPI QR</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
           <t>NRNS</t>
         </is>
       </c>
-      <c r="N54" t="inlineStr">
-        <is>
-          <t>783823510579</t>
-        </is>
-      </c>
-      <c r="O54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P54" t="inlineStr">
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>108557239779</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P55" t="inlineStr">
         <is>
           <t>100000036600</t>
         </is>
       </c>
-      <c r="Q54" t="inlineStr">
+      <c r="Q55" t="inlineStr">
         <is>
           <t>SIBL0000899</t>
         </is>
       </c>
-      <c r="R54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="S54" t="inlineStr">
+      <c r="R55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S55" t="inlineStr">
         <is>
           <t>MERCHANT</t>
         </is>
       </c>
-      <c r="T54" t="inlineStr">
+      <c r="T55" t="inlineStr">
         <is>
           <t>UPI</t>
         </is>
       </c>
-      <c r="U54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="V54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="W54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="X54" t="inlineStr">
-        <is>
-          <t>THUTTA DHANASHVI</t>
-        </is>
-      </c>
-      <c r="Y54" t="inlineStr">
+      <c r="U55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X55" t="inlineStr">
+        <is>
+          <t>VELAMALA RUTVIK VIHAAN</t>
+        </is>
+      </c>
+      <c r="Y55" t="inlineStr">
         <is>
           <t>kotakschoolvsp@gmail.com</t>
         </is>
       </c>
-      <c r="Z54" t="inlineStr">
-        <is>
-          <t>7337239208</t>
-        </is>
-      </c>
-      <c r="AA54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AB54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AC54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AD54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AE54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AF54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AG54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AH54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AI54" t="inlineStr">
+      <c r="Z55" t="inlineStr">
+        <is>
+          <t>9603662924</t>
+        </is>
+      </c>
+      <c r="AA55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI55" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="AJ54" t="inlineStr">
+      <c r="AJ55" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="AK54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AL54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AM54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AN54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AO54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AP54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AQ54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AR54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AS54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AT54" t="inlineStr">
+      <c r="AK55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT55" t="inlineStr">
         <is>
           <t>TRANSACTION IS SUCCESSFUL</t>
         </is>
       </c>
-      <c r="AU54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AV54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AW54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AX54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AY54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AZ54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BA54" t="inlineStr">
+      <c r="AU55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA55" t="inlineStr">
         <is>
           <t>UPI</t>
         </is>
       </c>
-      <c r="BB54" t="inlineStr">
+      <c r="BB55" t="inlineStr">
+        <is>
+          <t>KOTAK SALESIAN SCHOOL MANAGEMENT ACCOUNT</t>
+        </is>
+      </c>
+      <c r="BC55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BD55" t="inlineStr">
+        <is>
+          <t>REGULAR</t>
+        </is>
+      </c>
+      <c r="BE55" t="inlineStr">
+        <is>
+          <t>20052</t>
+        </is>
+      </c>
+      <c r="BF55" t="inlineStr">
+        <is>
+          <t>263452</t>
+        </is>
+      </c>
+      <c r="BG55" t="inlineStr">
+        <is>
+          <t>2039</t>
+        </is>
+      </c>
+      <c r="BH55" t="inlineStr">
+        <is>
+          <t>six thousand seven hundred fifty</t>
+        </is>
+      </c>
+      <c r="BI55" t="inlineStr">
+        <is>
+          <t>17337</t>
+        </is>
+      </c>
+      <c r="BJ55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BK55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BL55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BM55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BN55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BO55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BP55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BQ55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BR55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BS55" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BT55" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BU55" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="BV55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>SALESIAN EDUCATION SOCIETY</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>753702</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>11000316293921</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>1762923744</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>8350.00</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>12-Nov-2025 10:32:49</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>lVl</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>sale</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>ICICI UPI QR</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>NRNS</t>
+        </is>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>214127184653</t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P56" t="inlineStr">
+        <is>
+          <t>100000036600</t>
+        </is>
+      </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>SIBL0000899</t>
+        </is>
+      </c>
+      <c r="R56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S56" t="inlineStr">
+        <is>
+          <t>MERCHANT</t>
+        </is>
+      </c>
+      <c r="T56" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="U56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X56" t="inlineStr">
+        <is>
+          <t>PEDDINTI JASWANTH</t>
+        </is>
+      </c>
+      <c r="Y56" t="inlineStr">
+        <is>
+          <t>kotakschoolvsp@gmail.com</t>
+        </is>
+      </c>
+      <c r="Z56" t="inlineStr">
+        <is>
+          <t>9550130840</t>
+        </is>
+      </c>
+      <c r="AA56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI56" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AJ56" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AK56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT56" t="inlineStr">
+        <is>
+          <t>TRANSACTION IS SUCCESSFUL</t>
+        </is>
+      </c>
+      <c r="AU56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA56" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="BB56" t="inlineStr">
         <is>
           <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
         </is>
       </c>
-      <c r="BC54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BD54" t="inlineStr">
+      <c r="BC56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BD56" t="inlineStr">
         <is>
           <t>REGULAR</t>
         </is>
       </c>
-      <c r="BE54" t="inlineStr">
-        <is>
-          <t>18339</t>
-        </is>
-      </c>
-      <c r="BF54" t="inlineStr">
-        <is>
-          <t>265347</t>
-        </is>
-      </c>
-      <c r="BG54" t="inlineStr">
-        <is>
-          <t>2048</t>
-        </is>
-      </c>
-      <c r="BH54" t="inlineStr">
-        <is>
-          <t>seven thousand seven hundred fifty</t>
-        </is>
-      </c>
-      <c r="BI54" t="inlineStr">
-        <is>
-          <t>16927</t>
-        </is>
-      </c>
-      <c r="BJ54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BK54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BL54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BM54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BN54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BO54" t="inlineStr">
+      <c r="BE56" t="inlineStr">
+        <is>
+          <t>18814</t>
+        </is>
+      </c>
+      <c r="BF56" t="inlineStr">
+        <is>
+          <t>265854</t>
+        </is>
+      </c>
+      <c r="BG56" t="inlineStr">
+        <is>
+          <t>2050</t>
+        </is>
+      </c>
+      <c r="BH56" t="inlineStr">
+        <is>
+          <t>eight thousand three hundred fifty</t>
+        </is>
+      </c>
+      <c r="BI56" t="inlineStr">
+        <is>
+          <t>16211</t>
+        </is>
+      </c>
+      <c r="BJ56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BK56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BL56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BM56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BN56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BO56" t="inlineStr">
         <is>
           <t>UPI INTENT</t>
         </is>
       </c>
-      <c r="BP54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BQ54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BR54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BS54" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BT54" t="inlineStr">
+      <c r="BP56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BQ56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BR56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BS56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BT56" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="BU54" t="inlineStr">
+      <c r="BU56" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="BV54" t="inlineStr">
+      <c r="BV56" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
Update fee collection and reports with latest transactions
Added new fee collection records and updated payment statuses in daywise_fees_collection.csv, daywise_fees_collection_2025-26.csv, and fee_transcation_atom_report.csv. Adjusted student fee balances in fees_collection.csv to reflect recent payments. Updated related Excel and Power BI report files to include the latest data.
</commit_message>
<xml_diff>
--- a/output_data/atom_report.xlsx
+++ b/output_data/atom_report.xlsx
@@ -20293,7 +20293,7 @@
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>NRNS</t>
+          <t>RS</t>
         </is>
       </c>
       <c r="N55" t="inlineStr">
@@ -20318,7 +20318,7 @@
       </c>
       <c r="R55" t="inlineStr">
         <is>
-          <t/>
+          <t>13-Nov-2025 00:00:00</t>
         </is>
       </c>
       <c r="S55" t="inlineStr">
@@ -20393,12 +20393,12 @@
       </c>
       <c r="AG55" t="inlineStr">
         <is>
-          <t/>
+          <t>5</t>
         </is>
       </c>
       <c r="AH55" t="inlineStr">
         <is>
-          <t/>
+          <t>0.9</t>
         </is>
       </c>
       <c r="AI55" t="inlineStr">
@@ -20413,17 +20413,17 @@
       </c>
       <c r="AK55" t="inlineStr">
         <is>
-          <t/>
+          <t>5.9</t>
         </is>
       </c>
       <c r="AL55" t="inlineStr">
         <is>
-          <t/>
+          <t>6750.0</t>
         </is>
       </c>
       <c r="AM55" t="inlineStr">
         <is>
-          <t/>
+          <t>13-Nov-2025 00:00:00</t>
         </is>
       </c>
       <c r="AN55" t="inlineStr">
@@ -20665,310 +20665,1798 @@
       </c>
       <c r="M56" t="inlineStr">
         <is>
+          <t>RS</t>
+        </is>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>214127184653</t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P56" t="inlineStr">
+        <is>
+          <t>100000036600</t>
+        </is>
+      </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>SIBL0000899</t>
+        </is>
+      </c>
+      <c r="R56" t="inlineStr">
+        <is>
+          <t>13-Nov-2025 00:00:00</t>
+        </is>
+      </c>
+      <c r="S56" t="inlineStr">
+        <is>
+          <t>MERCHANT</t>
+        </is>
+      </c>
+      <c r="T56" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="U56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X56" t="inlineStr">
+        <is>
+          <t>PEDDINTI JASWANTH</t>
+        </is>
+      </c>
+      <c r="Y56" t="inlineStr">
+        <is>
+          <t>kotakschoolvsp@gmail.com</t>
+        </is>
+      </c>
+      <c r="Z56" t="inlineStr">
+        <is>
+          <t>9550130840</t>
+        </is>
+      </c>
+      <c r="AA56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG56" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AH56" t="inlineStr">
+        <is>
+          <t>0.9</t>
+        </is>
+      </c>
+      <c r="AI56" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AJ56" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AK56" t="inlineStr">
+        <is>
+          <t>5.9</t>
+        </is>
+      </c>
+      <c r="AL56" t="inlineStr">
+        <is>
+          <t>8350.0</t>
+        </is>
+      </c>
+      <c r="AM56" t="inlineStr">
+        <is>
+          <t>13-Nov-2025 00:00:00</t>
+        </is>
+      </c>
+      <c r="AN56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT56" t="inlineStr">
+        <is>
+          <t>TRANSACTION IS SUCCESSFUL</t>
+        </is>
+      </c>
+      <c r="AU56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA56" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="BB56" t="inlineStr">
+        <is>
+          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
+        </is>
+      </c>
+      <c r="BC56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BD56" t="inlineStr">
+        <is>
+          <t>REGULAR</t>
+        </is>
+      </c>
+      <c r="BE56" t="inlineStr">
+        <is>
+          <t>18814</t>
+        </is>
+      </c>
+      <c r="BF56" t="inlineStr">
+        <is>
+          <t>265854</t>
+        </is>
+      </c>
+      <c r="BG56" t="inlineStr">
+        <is>
+          <t>2050</t>
+        </is>
+      </c>
+      <c r="BH56" t="inlineStr">
+        <is>
+          <t>eight thousand three hundred fifty</t>
+        </is>
+      </c>
+      <c r="BI56" t="inlineStr">
+        <is>
+          <t>16211</t>
+        </is>
+      </c>
+      <c r="BJ56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BK56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BL56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BM56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BN56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BO56" t="inlineStr">
+        <is>
+          <t>UPI INTENT</t>
+        </is>
+      </c>
+      <c r="BP56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BQ56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BR56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BS56" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BT56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BU56" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="BV56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>SALESIAN EDUCATION SOCIETY</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>753702</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>11000316406420</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>1762965377</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>7750.00</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>12-Nov-2025 22:07:06</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>lVl</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>sale</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>ICICI UPI QR</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
           <t>NRNS</t>
         </is>
       </c>
-      <c r="N56" t="inlineStr">
-        <is>
-          <t>214127184653</t>
-        </is>
-      </c>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="P56" t="inlineStr">
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>108561533019</t>
+        </is>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P57" t="inlineStr">
         <is>
           <t>100000036600</t>
         </is>
       </c>
-      <c r="Q56" t="inlineStr">
+      <c r="Q57" t="inlineStr">
         <is>
           <t>SIBL0000899</t>
         </is>
       </c>
-      <c r="R56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="S56" t="inlineStr">
+      <c r="R57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S57" t="inlineStr">
         <is>
           <t>MERCHANT</t>
         </is>
       </c>
-      <c r="T56" t="inlineStr">
+      <c r="T57" t="inlineStr">
         <is>
           <t>UPI</t>
         </is>
       </c>
-      <c r="U56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="V56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="W56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="X56" t="inlineStr">
-        <is>
-          <t>PEDDINTI JASWANTH</t>
-        </is>
-      </c>
-      <c r="Y56" t="inlineStr">
+      <c r="U57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X57" t="inlineStr">
+        <is>
+          <t>GUNIPE NIHARIKA</t>
+        </is>
+      </c>
+      <c r="Y57" t="inlineStr">
         <is>
           <t>kotakschoolvsp@gmail.com</t>
         </is>
       </c>
-      <c r="Z56" t="inlineStr">
-        <is>
-          <t>9550130840</t>
-        </is>
-      </c>
-      <c r="AA56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AB56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AC56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AD56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AE56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AF56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AG56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AH56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AI56" t="inlineStr">
+      <c r="Z57" t="inlineStr">
+        <is>
+          <t>9966262514</t>
+        </is>
+      </c>
+      <c r="AA57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI57" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="AJ56" t="inlineStr">
+      <c r="AJ57" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="AK56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AL56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AM56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AN56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AO56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AP56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AQ56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AR56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AS56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AT56" t="inlineStr">
+      <c r="AK57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT57" t="inlineStr">
+        <is>
+          <t>TRANSACTION IS FAILED</t>
+        </is>
+      </c>
+      <c r="AU57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA57" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="BB57" t="inlineStr">
+        <is>
+          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
+        </is>
+      </c>
+      <c r="BC57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BD57" t="inlineStr">
+        <is>
+          <t>REGULAR</t>
+        </is>
+      </c>
+      <c r="BE57" t="inlineStr">
+        <is>
+          <t>19893</t>
+        </is>
+      </c>
+      <c r="BF57" t="inlineStr">
+        <is>
+          <t>265185</t>
+        </is>
+      </c>
+      <c r="BG57" t="inlineStr">
+        <is>
+          <t>2048</t>
+        </is>
+      </c>
+      <c r="BH57" t="inlineStr">
+        <is>
+          <t>seven thousand seven hundred fifty</t>
+        </is>
+      </c>
+      <c r="BI57" t="inlineStr">
+        <is>
+          <t>17178</t>
+        </is>
+      </c>
+      <c r="BJ57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BK57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BL57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BM57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BN57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BO57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BP57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BQ57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BR57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BS57" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BT57" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BU57" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="BV57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>SALESIAN EDUCATION SOCIETY</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>753702</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>11000316429828</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>1763001056</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>500.00</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>13-Nov-2025 08:04:29</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>lVl</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>sale</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>ICICI UPI QR</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>NRNS</t>
+        </is>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>108562616014</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P58" t="inlineStr">
+        <is>
+          <t>100000036600</t>
+        </is>
+      </c>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>SIBL0000899</t>
+        </is>
+      </c>
+      <c r="R58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S58" t="inlineStr">
+        <is>
+          <t>MERCHANT</t>
+        </is>
+      </c>
+      <c r="T58" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="U58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X58" t="inlineStr">
+        <is>
+          <t>THOKALA HRITVIK</t>
+        </is>
+      </c>
+      <c r="Y58" t="inlineStr">
+        <is>
+          <t>kotakschoolvsp@gmail.com</t>
+        </is>
+      </c>
+      <c r="Z58" t="inlineStr">
+        <is>
+          <t>9701283755</t>
+        </is>
+      </c>
+      <c r="AA58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI58" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AJ58" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AK58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT58" t="inlineStr">
+        <is>
+          <t>TRANSACTION IS FAILED</t>
+        </is>
+      </c>
+      <c r="AU58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA58" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="BB58" t="inlineStr">
+        <is>
+          <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
+        </is>
+      </c>
+      <c r="BC58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BD58" t="inlineStr">
+        <is>
+          <t>REGULAR</t>
+        </is>
+      </c>
+      <c r="BE58" t="inlineStr">
+        <is>
+          <t>19007</t>
+        </is>
+      </c>
+      <c r="BF58" t="inlineStr">
+        <is>
+          <t>262999</t>
+        </is>
+      </c>
+      <c r="BG58" t="inlineStr">
+        <is>
+          <t>2037</t>
+        </is>
+      </c>
+      <c r="BH58" t="inlineStr">
+        <is>
+          <t>five hundred</t>
+        </is>
+      </c>
+      <c r="BI58" t="inlineStr">
+        <is>
+          <t>16274</t>
+        </is>
+      </c>
+      <c r="BJ58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BK58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BL58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BM58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BN58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BO58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BP58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BQ58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BR58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BS58" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BT58" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BU58" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="BV58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>SALESIAN EDUCATION SOCIETY</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>753702</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>11000316431279</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>1763001959</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>7750.00</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>13-Nov-2025 08:16:51</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>lVl</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>sale</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>ICICI UPI QR</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>NRNS</t>
+        </is>
+      </c>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>108562669809</t>
+        </is>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P59" t="inlineStr">
+        <is>
+          <t>100000036600</t>
+        </is>
+      </c>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>SIBL0000899</t>
+        </is>
+      </c>
+      <c r="R59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S59" t="inlineStr">
+        <is>
+          <t>MERCHANT</t>
+        </is>
+      </c>
+      <c r="T59" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="U59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X59" t="inlineStr">
+        <is>
+          <t>TALACHINTALA SURYA NIMROD</t>
+        </is>
+      </c>
+      <c r="Y59" t="inlineStr">
+        <is>
+          <t>kotakschoolvsp@gmail.com</t>
+        </is>
+      </c>
+      <c r="Z59" t="inlineStr">
+        <is>
+          <t>9492203981</t>
+        </is>
+      </c>
+      <c r="AA59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI59" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AJ59" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AK59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT59" t="inlineStr">
         <is>
           <t>TRANSACTION IS SUCCESSFUL</t>
         </is>
       </c>
-      <c r="AU56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AV56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AW56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AX56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AY56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AZ56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BA56" t="inlineStr">
+      <c r="AU59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA59" t="inlineStr">
         <is>
           <t>UPI</t>
         </is>
       </c>
-      <c r="BB56" t="inlineStr">
+      <c r="BB59" t="inlineStr">
         <is>
           <t>KOTAK SALESIAN PRIMARY SCHOOL</t>
         </is>
       </c>
-      <c r="BC56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BD56" t="inlineStr">
+      <c r="BC59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BD59" t="inlineStr">
         <is>
           <t>REGULAR</t>
         </is>
       </c>
-      <c r="BE56" t="inlineStr">
-        <is>
-          <t>18814</t>
-        </is>
-      </c>
-      <c r="BF56" t="inlineStr">
-        <is>
-          <t>265854</t>
-        </is>
-      </c>
-      <c r="BG56" t="inlineStr">
-        <is>
-          <t>2050</t>
-        </is>
-      </c>
-      <c r="BH56" t="inlineStr">
-        <is>
-          <t>eight thousand three hundred fifty</t>
-        </is>
-      </c>
-      <c r="BI56" t="inlineStr">
-        <is>
-          <t>16211</t>
-        </is>
-      </c>
-      <c r="BJ56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BK56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BL56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BM56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BN56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BO56" t="inlineStr">
+      <c r="BE59" t="inlineStr">
+        <is>
+          <t>18172</t>
+        </is>
+      </c>
+      <c r="BF59" t="inlineStr">
+        <is>
+          <t>265254</t>
+        </is>
+      </c>
+      <c r="BG59" t="inlineStr">
+        <is>
+          <t>2048</t>
+        </is>
+      </c>
+      <c r="BH59" t="inlineStr">
+        <is>
+          <t>seven thousand seven hundred fifty</t>
+        </is>
+      </c>
+      <c r="BI59" t="inlineStr">
+        <is>
+          <t>16648</t>
+        </is>
+      </c>
+      <c r="BJ59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BK59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BL59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BM59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BN59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BO59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BP59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BQ59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BR59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BS59" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BT59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BU59" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="BV59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>SALESIAN EDUCATION SOCIETY</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>753702</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>11000316535819</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>1763035319</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>6750.00</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>13-Nov-2025 17:32:13</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>PREKGUKG</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>sale</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>ICICI UPI QR</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>NRNS</t>
+        </is>
+      </c>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t>173230421882</t>
+        </is>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="P60" t="inlineStr">
+        <is>
+          <t>100000036600</t>
+        </is>
+      </c>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>SIBL0000899</t>
+        </is>
+      </c>
+      <c r="R60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S60" t="inlineStr">
+        <is>
+          <t>MERCHANT</t>
+        </is>
+      </c>
+      <c r="T60" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="U60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="V60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X60" t="inlineStr">
+        <is>
+          <t>CHINTHA VAISHNAVI</t>
+        </is>
+      </c>
+      <c r="Y60" t="inlineStr">
+        <is>
+          <t>kotakschoolvsp@gmail.com</t>
+        </is>
+      </c>
+      <c r="Z60" t="inlineStr">
+        <is>
+          <t>8886428971</t>
+        </is>
+      </c>
+      <c r="AA60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AC60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AD60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AE60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AF60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AG60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AH60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AI60" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AJ60" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AK60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AL60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AM60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AN60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AO60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AP60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AQ60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AR60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AS60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AT60" t="inlineStr">
+        <is>
+          <t>TRANSACTION IS SUCCESSFUL</t>
+        </is>
+      </c>
+      <c r="AU60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AV60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AW60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AX60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AY60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AZ60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BA60" t="inlineStr">
+        <is>
+          <t>UPI</t>
+        </is>
+      </c>
+      <c r="BB60" t="inlineStr">
+        <is>
+          <t>KOTAK SALESIAN SCHOOL MANAGEMENT ACCOUNT</t>
+        </is>
+      </c>
+      <c r="BC60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BD60" t="inlineStr">
+        <is>
+          <t>REGULAR</t>
+        </is>
+      </c>
+      <c r="BE60" t="inlineStr">
+        <is>
+          <t>19901</t>
+        </is>
+      </c>
+      <c r="BF60" t="inlineStr">
+        <is>
+          <t>264986</t>
+        </is>
+      </c>
+      <c r="BG60" t="inlineStr">
+        <is>
+          <t>2047</t>
+        </is>
+      </c>
+      <c r="BH60" t="inlineStr">
+        <is>
+          <t>six thousand seven hundred fifty</t>
+        </is>
+      </c>
+      <c r="BI60" t="inlineStr">
+        <is>
+          <t>17187</t>
+        </is>
+      </c>
+      <c r="BJ60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BK60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BL60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BM60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BN60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BO60" t="inlineStr">
         <is>
           <t>UPI INTENT</t>
         </is>
       </c>
-      <c r="BP56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BQ56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BR56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BS56" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="BT56" t="inlineStr">
+      <c r="BP60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BQ60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BR60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BS60" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="BT60" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="BU56" t="inlineStr">
+      <c r="BU60" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="BV56" t="inlineStr">
+      <c r="BV60" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>